<commit_message>
Updated Desktop-UI & Server
</commit_message>
<xml_diff>
--- a/Benötigte Teile.xlsx
+++ b/Benötigte Teile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="28800" windowHeight="12345" xr2:uid="{8EDA0229-25EB-4497-B30B-53A3F84FB94C}"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="28800" windowHeight="12345" xr2:uid="{8EDA0229-25EB-4497-B30B-53A3F84FB94C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Pi Zero W</t>
   </si>
   <si>
-    <t>https://www.amazon.de/dp/B06XCYGP27</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
@@ -56,16 +53,22 @@
     <t>Sensor</t>
   </si>
   <si>
-    <t>https://www.ebay.de/itm/173031445980</t>
-  </si>
-  <si>
-    <t>https://www.ebay.de/itm/273139527827</t>
-  </si>
-  <si>
     <t>Kinect v2</t>
   </si>
   <si>
     <t>Kinect v2 Adapter</t>
+  </si>
+  <si>
+    <t>Gesamt</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/dp/B0798NK28L/</t>
+  </si>
+  <si>
+    <t>Glühbirne</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/dp/B06XCYGP27/</t>
   </si>
 </sst>
 </file>
@@ -429,7 +432,7 @@
   <dimension ref="B2:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,16 +444,16 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -458,10 +461,10 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1">
         <v>25</v>
@@ -469,13 +472,13 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
       </c>
       <c r="E4" s="1">
         <v>4</v>
@@ -483,34 +486,39 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
       <c r="E5" s="1">
-        <v>110</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1">
-        <v>65</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E7" s="2"/>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1">
+        <v>70</v>
+      </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E8" s="2"/>
@@ -534,7 +542,13 @@
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E15" s="2"/>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="1">
+        <f>SUM(E3:E9)</f>
+        <v>221</v>
+      </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E16" s="2"/>

</xml_diff>